<commit_message>
Fix board outline Gerbers
</commit_message>
<xml_diff>
--- a/Project Outputs for Magnetic-Sequencer/BOM/Bill of Materials-Magnetic-Sequencer.xlsx
+++ b/Project Outputs for Magnetic-Sequencer/BOM/Bill of Materials-Magnetic-Sequencer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\x-io\Open-Source\Magnetic-Sequencer\Project Outputs for Magnetic-Sequencer\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{588CF30E-A012-4066-935E-5E58B990638C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B344B10B-A19B-4D74-ADF7-B9C71EECEE8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23745" yWindow="8985" windowWidth="20190" windowHeight="15435" xr2:uid="{5E9277BF-13B3-47B4-B091-39DC4C2501D3}"/>
+    <workbookView xWindow="-15390" yWindow="10875" windowWidth="14400" windowHeight="13185" xr2:uid="{737E54D0-6BF1-4804-AFDC-06C674F21A9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Magnetic-Sequ" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
     <t>R1, R19, R20</t>
   </si>
   <si>
-    <t>5.1k, 0603</t>
+    <t>5.1kR, 0603</t>
   </si>
   <si>
     <t>Resistor 0603</t>
@@ -118,7 +118,7 @@
     <t>R3, R4, R5, R6, R7, R8, R9, R10</t>
   </si>
   <si>
-    <t>1.2k, 0603</t>
+    <t>1.2kR, 0603</t>
   </si>
   <si>
     <t>R21</t>
@@ -548,7 +548,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68601C60-46BF-4927-AD0A-FF5257FC01F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE94564-205F-43CC-854F-1C1256838168}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>